<commit_message>
Modified the sprint burn-down excel
</commit_message>
<xml_diff>
--- a/Scrum/SPRINT BACKLOG/SprintBacklog.xlsx
+++ b/Scrum/SPRINT BACKLOG/SprintBacklog.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Itumeleng Malematja\Desktop\COMPUTER SCIENCE\COS301\FINAL PROJECT\COEUS\ADMIN\SPRINT BACKLOG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Itumeleng Malematja\Desktop\COMPUTER SCIENCE\COS301\FINAL PROJECT\COEUS\GeospatialDataProcessorVisualiser_documentation\Scrum\SPRINT BACKLOG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -535,51 +536,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -650,6 +609,48 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,6 +683,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ZA"/>
+              <a:t>Sprint no.1 Burn-down</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -744,6 +770,56 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$3:$R$3</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$23:$R$23</c:f>
@@ -826,6 +902,56 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$3:$R$3</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Day 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Day 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Day 10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Day 11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Day 12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Day 13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Day 14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$24:$R$24</c:f>
@@ -891,16 +1017,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1047369472"/>
-        <c:axId val="1047371648"/>
+        <c:axId val="1623409648"/>
+        <c:axId val="1623411824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1047369472"/>
+        <c:axId val="1623409648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -937,7 +1064,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1047371648"/>
+        <c:crossAx val="1623411824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -945,7 +1072,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1047371648"/>
+        <c:axId val="1623411824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -965,6 +1092,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-ZA"/>
+                  <a:t>Time(hr)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -996,7 +1179,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1047369472"/>
+        <c:crossAx val="1623409648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1069,11 +1252,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1633,25 +1811,28 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>971550</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1664,7 +1845,7 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1933,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,751 +2128,751 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="12"/>
-      <c r="T2" s="20" t="s">
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="T2" s="34" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="15" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="Q3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="R3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="21"/>
+      <c r="T3" s="35"/>
     </row>
     <row r="4" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="36" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="35">
+      <c r="D4" s="21">
         <v>20</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="22">
         <v>3</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="23">
         <v>2</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="23">
         <v>3</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="23">
         <v>1</v>
       </c>
-      <c r="I4" s="37">
+      <c r="I4" s="23">
         <v>6</v>
       </c>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37">
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23">
         <v>3</v>
       </c>
-      <c r="Q4" s="37">
+      <c r="Q4" s="23">
         <v>2</v>
       </c>
-      <c r="R4" s="38"/>
-      <c r="T4" s="22">
+      <c r="R4" s="24"/>
+      <c r="T4" s="8">
         <f>SUM(E4:R4)</f>
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="25">
         <v>10</v>
       </c>
-      <c r="E5" s="36">
+      <c r="E5" s="22">
         <v>2</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="26">
         <v>3</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G5" s="26">
         <v>3</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5" s="26">
         <v>3</v>
       </c>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="38"/>
-      <c r="T5" s="22">
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="24"/>
+      <c r="T5" s="8">
         <f>SUM(E5:R5)</f>
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D6" s="25">
         <v>1</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="38">
+      <c r="E6" s="22"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="24">
         <v>3</v>
       </c>
-      <c r="T6" s="22">
+      <c r="T6" s="8">
         <f t="shared" ref="T6:T21" si="0">SUM(E6:R6)</f>
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="25">
         <v>2</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="22">
         <v>2</v>
       </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="38"/>
-      <c r="T7" s="22">
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="24"/>
+      <c r="T7" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:20" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="7"/>
-      <c r="C8" s="46" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="25">
         <v>1</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="40"/>
-      <c r="R8" s="38">
+      <c r="E8" s="22"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="24">
         <v>1</v>
       </c>
-      <c r="T8" s="22"/>
+      <c r="T8" s="8"/>
     </row>
     <row r="9" spans="2:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="21">
         <v>20</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
       <c r="J9" s="1">
         <v>5</v>
       </c>
-      <c r="K9" s="37">
+      <c r="K9" s="23">
         <v>4</v>
       </c>
-      <c r="L9" s="37">
+      <c r="L9" s="23">
         <v>4</v>
       </c>
-      <c r="M9" s="37">
+      <c r="M9" s="23">
         <v>3</v>
       </c>
-      <c r="N9" s="37">
+      <c r="N9" s="23">
         <v>4</v>
       </c>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="41"/>
-      <c r="T9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="27"/>
+      <c r="T9" s="9"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="25">
         <v>3</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="40">
+      <c r="E10" s="22"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="26">
         <v>1</v>
       </c>
-      <c r="L10" s="40">
+      <c r="L10" s="26">
         <v>2</v>
       </c>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="38"/>
-      <c r="T10" s="22"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="24"/>
+      <c r="T10" s="8"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="25">
         <v>2</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40">
+      <c r="E11" s="22"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26">
         <v>1</v>
       </c>
-      <c r="N11" s="40">
+      <c r="N11" s="26">
         <v>1</v>
       </c>
-      <c r="O11" s="40"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="38"/>
-      <c r="T11" s="22"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="24"/>
+      <c r="T11" s="8"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="39">
+      <c r="D12" s="25">
         <v>1</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40">
+      <c r="E12" s="22"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26">
         <v>1</v>
       </c>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="38"/>
-      <c r="T12" s="22">
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="24"/>
+      <c r="T12" s="8">
         <f>SUM(E12:R12)</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="40"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="38"/>
-      <c r="T13" s="22">
+      <c r="D13" s="25"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="24"/>
+      <c r="T13" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="44"/>
-      <c r="P14" s="44"/>
-      <c r="Q14" s="44"/>
-      <c r="R14" s="45"/>
-      <c r="T14" s="22">
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="31"/>
+      <c r="T14" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="36" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="21">
         <v>2</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37">
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23">
         <v>1</v>
       </c>
-      <c r="J15" s="37">
+      <c r="J15" s="23">
         <v>1</v>
       </c>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="41"/>
-      <c r="T15" s="23">
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="27"/>
+      <c r="T15" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D16" s="25">
         <v>3</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40">
+      <c r="E16" s="22"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26">
         <v>1</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40">
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26">
         <v>2</v>
       </c>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="40"/>
-      <c r="P16" s="40"/>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="38"/>
-      <c r="T16" s="22">
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="24"/>
+      <c r="T16" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="39">
+      <c r="D17" s="25">
         <v>2</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40">
+      <c r="E17" s="22"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26">
         <v>2</v>
       </c>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="38"/>
-      <c r="T17" s="22">
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="24"/>
+      <c r="T17" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="39">
+      <c r="D18" s="25">
         <v>4</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40">
+      <c r="E18" s="22"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26">
         <v>1</v>
       </c>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40">
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26">
         <v>2</v>
       </c>
-      <c r="N18" s="40">
+      <c r="N18" s="26">
         <v>1</v>
       </c>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="38"/>
-      <c r="T18" s="22">
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="24"/>
+      <c r="T18" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="39">
+      <c r="D19" s="25">
         <v>24</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40">
+      <c r="E19" s="22"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26">
         <v>2</v>
       </c>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40">
+      <c r="K19" s="26"/>
+      <c r="L19" s="26">
         <v>3</v>
       </c>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40">
+      <c r="M19" s="26"/>
+      <c r="N19" s="26">
         <v>5</v>
       </c>
-      <c r="O19" s="40">
+      <c r="O19" s="26">
         <v>6</v>
       </c>
-      <c r="P19" s="40">
+      <c r="P19" s="26">
         <v>2</v>
       </c>
-      <c r="Q19" s="40">
+      <c r="Q19" s="26">
         <v>2</v>
       </c>
-      <c r="R19" s="38"/>
-      <c r="T19" s="22">
+      <c r="R19" s="24"/>
+      <c r="T19" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="38"/>
-      <c r="T20" s="22">
+      <c r="D20" s="25"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="24"/>
+      <c r="T20" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="7"/>
+      <c r="B21" s="38"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="44"/>
-      <c r="Q21" s="44"/>
-      <c r="R21" s="45"/>
-      <c r="T21" s="24">
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="31"/>
+      <c r="T21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="13">
         <f>SUM(D4:D21)</f>
         <v>95</v>
       </c>
-      <c r="E23" s="28">
-        <f>D23-SUM(E4:E21)</f>
+      <c r="E23" s="14">
+        <f t="shared" ref="E23:R23" si="1">D23-SUM(E4:E21)</f>
         <v>88</v>
       </c>
-      <c r="F23" s="29">
-        <f>E23-SUM(F4:F21)</f>
+      <c r="F23" s="15">
+        <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="G23" s="29">
-        <f>F23-SUM(G4:G21)</f>
+      <c r="G23" s="15">
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="H23" s="29">
-        <f>G23-SUM(H4:H21)</f>
+      <c r="H23" s="15">
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="I23" s="29">
-        <f>H23-SUM(I4:I21)</f>
+      <c r="I23" s="15">
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="J23" s="29">
-        <f>I23-SUM(J4:J21)</f>
+      <c r="J23" s="15">
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="K23" s="29">
-        <f>J23-SUM(K4:K21)</f>
+      <c r="K23" s="15">
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="L23" s="29">
-        <f>K23-SUM(L4:L21)</f>
+      <c r="L23" s="15">
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="M23" s="29">
-        <f>L23-SUM(M4:M21)</f>
+      <c r="M23" s="15">
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="N23" s="29">
-        <f>M23-SUM(N4:N21)</f>
+      <c r="N23" s="15">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="O23" s="29">
-        <f>N23-SUM(O4:O21)</f>
+      <c r="O23" s="15">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="P23" s="29">
-        <f>O23-SUM(P4:P21)</f>
+      <c r="P23" s="15">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="Q23" s="29">
-        <f>P23-SUM(Q4:Q21)</f>
+      <c r="Q23" s="15">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="R23" s="30">
-        <f>Q23-SUM(R4:R21)</f>
+      <c r="R23" s="16">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="17">
         <f>SUM(D4:D21)</f>
         <v>95</v>
       </c>
-      <c r="E24" s="32">
-        <f>D24-($D$24/14)</f>
+      <c r="E24" s="18">
+        <f t="shared" ref="E24:R24" si="2">D24-($D$24/14)</f>
         <v>88.214285714285708</v>
       </c>
-      <c r="F24" s="33">
-        <f>E24-($D$24/14)</f>
+      <c r="F24" s="19">
+        <f t="shared" si="2"/>
         <v>81.428571428571416</v>
       </c>
-      <c r="G24" s="33">
-        <f>F24-($D$24/14)</f>
+      <c r="G24" s="19">
+        <f t="shared" si="2"/>
         <v>74.642857142857125</v>
       </c>
-      <c r="H24" s="33">
-        <f>G24-($D$24/14)</f>
+      <c r="H24" s="19">
+        <f t="shared" si="2"/>
         <v>67.857142857142833</v>
       </c>
-      <c r="I24" s="33">
-        <f>H24-($D$24/14)</f>
+      <c r="I24" s="19">
+        <f t="shared" si="2"/>
         <v>61.071428571428548</v>
       </c>
-      <c r="J24" s="33">
-        <f>I24-($D$24/14)</f>
+      <c r="J24" s="19">
+        <f t="shared" si="2"/>
         <v>54.285714285714263</v>
       </c>
-      <c r="K24" s="33">
-        <f>J24-($D$24/14)</f>
+      <c r="K24" s="19">
+        <f t="shared" si="2"/>
         <v>47.499999999999979</v>
       </c>
-      <c r="L24" s="33">
-        <f>K24-($D$24/14)</f>
+      <c r="L24" s="19">
+        <f t="shared" si="2"/>
         <v>40.714285714285694</v>
       </c>
-      <c r="M24" s="33">
-        <f>L24-($D$24/14)</f>
+      <c r="M24" s="19">
+        <f t="shared" si="2"/>
         <v>33.928571428571409</v>
       </c>
-      <c r="N24" s="33">
-        <f>M24-($D$24/14)</f>
+      <c r="N24" s="19">
+        <f t="shared" si="2"/>
         <v>27.142857142857125</v>
       </c>
-      <c r="O24" s="33">
-        <f>N24-($D$24/14)</f>
+      <c r="O24" s="19">
+        <f t="shared" si="2"/>
         <v>20.35714285714284</v>
       </c>
-      <c r="P24" s="33">
-        <f>O24-($D$24/14)</f>
+      <c r="P24" s="19">
+        <f t="shared" si="2"/>
         <v>13.571428571428555</v>
       </c>
-      <c r="Q24" s="33">
-        <f>P24-($D$24/14)</f>
+      <c r="Q24" s="19">
+        <f t="shared" si="2"/>
         <v>6.7857142857142696</v>
       </c>
-      <c r="R24" s="34">
-        <f>Q24-($D$24/14)</f>
+      <c r="R24" s="20">
+        <f t="shared" si="2"/>
         <v>-1.5987211554602254E-14</v>
       </c>
     </row>
@@ -2707,6 +2888,5 @@
     <mergeCell ref="D2:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>